<commit_message>
insert data into multiple worksheets in excel
</commit_message>
<xml_diff>
--- a/insertDataIntoExcell-python/sample.xlsx
+++ b/insertDataIntoExcell-python/sample.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMD\Desktop\HatGuy68\Mini-Projects\insertDataIntoExcell-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913A141-DAD9-4DC6-BF46-455F8EA3F060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EE5709-230F-4476-B55B-337FD13AAC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Patient Records" sheetId="1" r:id="rId1"/>
+    <sheet name="Medications" sheetId="2" r:id="rId2"/>
+    <sheet name="Activities" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>S.No.</t>
   </si>
@@ -37,43 +39,49 @@
     <t>Condition</t>
   </si>
   <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>heart failure</t>
+  </si>
+  <si>
+    <t>Patient No.</t>
+  </si>
+  <si>
     <t>Medication</t>
   </si>
   <si>
+    <t>blood-thinner</t>
+  </si>
+  <si>
+    <t>thomapyrin</t>
+  </si>
+  <si>
+    <t>Aspirin</t>
+  </si>
+  <si>
     <t>Activities</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Nair</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>heart failure</t>
-  </si>
-  <si>
-    <t>blood-thinner thomapyrin Aspirin</t>
-  </si>
-  <si>
-    <t>blood-pressure Pulse-rate blood-sugar-levels Blood-drawn</t>
-  </si>
-  <si>
-    <t>['blood-thinner', 'thomapyrin', 'Aspirin']</t>
-  </si>
-  <si>
-    <t>['blood-pressure', 'Pulse-rate', 'blood-sugar-levels', 'Blood-drawn']</t>
+    <t>blood-pressure</t>
+  </si>
+  <si>
+    <t>Pulse-rate</t>
+  </si>
+  <si>
+    <t>blood-sugar-levels</t>
+  </si>
+  <si>
+    <t>Blood-drawn</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -425,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +449,7 @@
     <col min="7" max="7" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,108 +465,176 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>